<commit_message>
Fri Sep  8 06:17:02 PM CST 2023
</commit_message>
<xml_diff>
--- a/lixiao/performance_2023_07/assess_绩效+软性考核表.xlsx
+++ b/lixiao/performance_2023_07/assess_绩效+软性考核表.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="28800" windowHeight="11310"/>
+    <workbookView windowWidth="28800" windowHeight="11355"/>
   </bookViews>
   <sheets>
     <sheet name="绩效表" sheetId="1" r:id="rId1"/>
@@ -836,10 +836,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
+    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
   </numFmts>
   <fonts count="37">
     <font>
@@ -927,6 +927,121 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="13"/>
       <color theme="3"/>
@@ -935,49 +1050,17 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
       <sz val="11"/>
-      <color rgb="FF800080"/>
+      <color rgb="FF3F3F76"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
       <sz val="11"/>
-      <color rgb="FF0000FF"/>
+      <color rgb="FF9C0006"/>
       <name val="Calibri"/>
       <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -989,89 +1072,6 @@
     </font>
     <font>
       <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
       <sz val="7"/>
       <color theme="1"/>
       <name val="Times New Roman"/>
@@ -1143,175 +1143,175 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFC6EFCE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1386,11 +1386,17 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1400,21 +1406,6 @@
       <top/>
       <bottom style="medium">
         <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1451,10 +1442,8 @@
     <border>
       <left/>
       <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
+      <top/>
+      <bottom style="medium">
         <color theme="4"/>
       </bottom>
       <diagonal/>
@@ -1469,182 +1458,193 @@
       <diagonal/>
     </border>
     <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
       </top>
       <bottom style="double">
-        <color rgb="FF3F3F3F"/>
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
       </bottom>
       <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="56">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="13" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="11" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="13" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="18" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="0" borderId="12" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="12" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="12" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="8" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="31" borderId="13" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="12" borderId="13" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="21" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="17" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="11" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="8" borderId="10" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="9" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="10" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="8" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="29" fillId="22" borderId="13" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="7" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="48">
+  <cellXfs count="54">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1735,6 +1735,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="49" fontId="3" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1744,24 +1750,36 @@
     <xf numFmtId="0" fontId="3" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="49" fontId="4" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="2" xfId="17" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="5" fillId="4" borderId="2" xfId="17" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="4" borderId="2" xfId="17" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="12" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="6" fillId="0" borderId="2" xfId="12" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="17" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="12" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="4" fillId="0" borderId="2" xfId="12" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="49" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="49" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
@@ -1782,8 +1800,8 @@
   </cellXfs>
   <cellStyles count="56">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="常规 14 2 2" xfId="1"/>
-    <cellStyle name="常规 2 2 2 2" xfId="2"/>
+    <cellStyle name="常规 2 2 2 2" xfId="1"/>
+    <cellStyle name="常规 14 2 2" xfId="2"/>
     <cellStyle name="60% - Accent6" xfId="3" builtinId="52"/>
     <cellStyle name="40% - Accent6" xfId="4" builtinId="51"/>
     <cellStyle name="60% - Accent5" xfId="5" builtinId="48"/>
@@ -1869,8 +1887,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="1918335" y="4257675"/>
-          <a:ext cx="15278100" cy="2781300"/>
+          <a:off x="1781175" y="4257675"/>
+          <a:ext cx="13506450" cy="2781300"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1929,8 +1947,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="11337925" y="3267075"/>
-          <a:ext cx="2338705" cy="533400"/>
+          <a:off x="10182225" y="3267075"/>
+          <a:ext cx="2019300" cy="533400"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2002,7 +2020,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="11909425" y="3857625"/>
+          <a:off x="10753725" y="3857625"/>
           <a:ext cx="323850" cy="581025"/>
         </a:xfrm>
         <a:prstGeom prst="upArrow">
@@ -2329,19 +2347,19 @@
   <dimension ref="A1:K40"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="K8" sqref="K8"/>
+      <selection activeCell="G11" sqref="G11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
   <cols>
-    <col min="2" max="2" width="5.37777777777778" customWidth="1"/>
-    <col min="3" max="3" width="14.5037037037037" customWidth="1"/>
-    <col min="4" max="4" width="9.62222222222222" customWidth="1"/>
+    <col min="2" max="2" width="5.375" customWidth="1"/>
+    <col min="3" max="3" width="14.5" customWidth="1"/>
+    <col min="4" max="4" width="9.625" customWidth="1"/>
     <col min="5" max="5" width="9" style="19" customWidth="1"/>
     <col min="6" max="6" width="15" customWidth="1"/>
-    <col min="7" max="8" width="29.3777777777778" customWidth="1"/>
-    <col min="9" max="9" width="33.5037037037037" customWidth="1"/>
-    <col min="10" max="10" width="27.5037037037037" customWidth="1"/>
+    <col min="7" max="8" width="29.375" customWidth="1"/>
+    <col min="9" max="9" width="33.5" customWidth="1"/>
+    <col min="10" max="10" width="27.5" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" ht="33" customHeight="1" spans="1:11">
@@ -2351,7 +2369,7 @@
       <c r="B1" s="20"/>
       <c r="C1" s="20"/>
       <c r="D1" s="20"/>
-      <c r="E1" s="20"/>
+      <c r="E1" s="32"/>
       <c r="F1" s="20"/>
       <c r="G1" s="20"/>
       <c r="H1" s="20"/>
@@ -2366,7 +2384,7 @@
       <c r="B3" s="21"/>
       <c r="C3" s="21"/>
       <c r="D3" s="21"/>
-      <c r="E3" s="21"/>
+      <c r="E3" s="33"/>
       <c r="F3" s="21"/>
       <c r="G3" s="21"/>
       <c r="H3" s="21"/>
@@ -2387,16 +2405,16 @@
       <c r="D5" s="22" t="s">
         <v>5</v>
       </c>
-      <c r="E5" s="32" t="s">
+      <c r="E5" s="34" t="s">
         <v>6</v>
       </c>
       <c r="F5" s="22" t="s">
         <v>7</v>
       </c>
-      <c r="G5" s="33" t="s">
+      <c r="G5" s="35" t="s">
         <v>8</v>
       </c>
-      <c r="H5" s="33"/>
+      <c r="H5" s="35"/>
       <c r="I5" s="22" t="s">
         <v>9</v>
       </c>
@@ -2412,12 +2430,12 @@
       <c r="B6" s="22"/>
       <c r="C6" s="22"/>
       <c r="D6" s="22"/>
-      <c r="E6" s="32"/>
+      <c r="E6" s="34"/>
       <c r="F6" s="22"/>
       <c r="G6" s="22" t="s">
         <v>12</v>
       </c>
-      <c r="H6" s="34" t="s">
+      <c r="H6" s="36" t="s">
         <v>13</v>
       </c>
       <c r="I6" s="22"/>
@@ -2437,16 +2455,16 @@
       <c r="D7" s="23" t="s">
         <v>16</v>
       </c>
-      <c r="E7" s="23"/>
+      <c r="E7" s="37"/>
       <c r="F7" s="23"/>
-      <c r="G7" s="35" t="s">
+      <c r="G7" s="38" t="s">
         <v>17</v>
       </c>
-      <c r="H7" s="36"/>
+      <c r="H7" s="39"/>
       <c r="I7" s="23" t="s">
         <v>18</v>
       </c>
-      <c r="J7" s="42" t="s">
+      <c r="J7" s="48" t="s">
         <v>19</v>
       </c>
       <c r="K7" s="23">
@@ -2466,12 +2484,12 @@
       <c r="D8" s="23" t="s">
         <v>16</v>
       </c>
-      <c r="E8" s="23"/>
+      <c r="E8" s="37"/>
       <c r="F8" s="23"/>
-      <c r="G8" s="35" t="s">
+      <c r="G8" s="38" t="s">
         <v>21</v>
       </c>
-      <c r="H8" s="36"/>
+      <c r="H8" s="39"/>
       <c r="I8" s="23" t="s">
         <v>18</v>
       </c>
@@ -2485,10 +2503,10 @@
       <c r="B9" s="23"/>
       <c r="C9" s="23"/>
       <c r="D9" s="23"/>
-      <c r="E9" s="23"/>
+      <c r="E9" s="37"/>
       <c r="F9" s="23"/>
-      <c r="G9" s="35"/>
-      <c r="H9" s="36"/>
+      <c r="G9" s="38"/>
+      <c r="H9" s="39"/>
       <c r="I9" s="23"/>
       <c r="J9" s="23"/>
       <c r="K9" s="23"/>
@@ -2498,12 +2516,12 @@
       <c r="B10" s="23"/>
       <c r="C10" s="23"/>
       <c r="D10" s="23"/>
-      <c r="E10" s="23"/>
+      <c r="E10" s="37"/>
       <c r="F10" s="23"/>
-      <c r="G10" s="35"/>
-      <c r="H10" s="36"/>
+      <c r="G10" s="38"/>
+      <c r="H10" s="39"/>
       <c r="I10" s="23"/>
-      <c r="J10" s="42"/>
+      <c r="J10" s="48"/>
       <c r="K10" s="23"/>
     </row>
     <row r="11" spans="1:11">
@@ -2511,7 +2529,7 @@
       <c r="B11" s="23"/>
       <c r="C11" s="23"/>
       <c r="D11" s="23"/>
-      <c r="E11" s="23"/>
+      <c r="E11" s="37"/>
       <c r="F11" s="23"/>
       <c r="G11" s="23"/>
       <c r="H11" s="23"/>
@@ -2524,7 +2542,7 @@
       <c r="B12" s="23"/>
       <c r="C12" s="23"/>
       <c r="D12" s="23"/>
-      <c r="E12" s="23"/>
+      <c r="E12" s="37"/>
       <c r="F12" s="23"/>
       <c r="G12" s="23"/>
       <c r="H12" s="23"/>
@@ -2541,25 +2559,25 @@
       <c r="D27" s="24" t="s">
         <v>23</v>
       </c>
-      <c r="E27" s="37" t="s">
+      <c r="E27" s="40" t="s">
         <v>24</v>
       </c>
       <c r="F27" s="24" t="s">
         <v>25</v>
       </c>
-      <c r="G27" s="38" t="s">
+      <c r="G27" s="41" t="s">
         <v>26</v>
       </c>
       <c r="H27" s="24" t="s">
         <v>27</v>
       </c>
-      <c r="I27" s="43" t="s">
+      <c r="I27" s="49" t="s">
         <v>28</v>
       </c>
-      <c r="J27" s="44" t="s">
+      <c r="J27" s="50" t="s">
         <v>29</v>
       </c>
-      <c r="K27" s="44" t="s">
+      <c r="K27" s="50" t="s">
         <v>30</v>
       </c>
     </row>
@@ -2567,10 +2585,10 @@
       <c r="D28" s="25" t="s">
         <v>31</v>
       </c>
-      <c r="E28" s="39" t="s">
+      <c r="E28" s="42" t="s">
         <v>32</v>
       </c>
-      <c r="F28" s="40" t="s">
+      <c r="F28" s="43" t="s">
         <v>33</v>
       </c>
       <c r="G28" s="26">
@@ -2579,18 +2597,18 @@
       <c r="H28" s="26">
         <v>1.1</v>
       </c>
-      <c r="I28" s="45" t="s">
+      <c r="I28" s="51" t="s">
         <v>34</v>
       </c>
       <c r="J28" s="26"/>
-      <c r="K28" s="46"/>
+      <c r="K28" s="52"/>
     </row>
     <row r="29" spans="4:11">
       <c r="D29" s="26"/>
-      <c r="E29" s="41" t="s">
+      <c r="E29" s="44" t="s">
         <v>35</v>
       </c>
-      <c r="F29" s="40" t="s">
+      <c r="F29" s="43" t="s">
         <v>36</v>
       </c>
       <c r="G29" s="26" t="s">
@@ -2599,20 +2617,20 @@
       <c r="H29" s="26" t="s">
         <v>38</v>
       </c>
-      <c r="I29" s="45" t="s">
+      <c r="I29" s="51" t="s">
         <v>39</v>
       </c>
       <c r="J29" s="26"/>
-      <c r="K29" s="46"/>
+      <c r="K29" s="52"/>
     </row>
     <row r="30" spans="4:11">
       <c r="D30" s="25" t="s">
         <v>40</v>
       </c>
-      <c r="E30" s="39" t="s">
+      <c r="E30" s="42" t="s">
         <v>32</v>
       </c>
-      <c r="F30" s="40" t="s">
+      <c r="F30" s="43" t="s">
         <v>33</v>
       </c>
       <c r="G30" s="26">
@@ -2621,18 +2639,18 @@
       <c r="H30" s="26">
         <v>1</v>
       </c>
-      <c r="I30" s="45" t="s">
+      <c r="I30" s="51" t="s">
         <v>41</v>
       </c>
       <c r="J30" s="26"/>
-      <c r="K30" s="47"/>
+      <c r="K30" s="53"/>
     </row>
     <row r="31" spans="4:11">
       <c r="D31" s="26"/>
-      <c r="E31" s="41" t="s">
+      <c r="E31" s="44" t="s">
         <v>35</v>
       </c>
-      <c r="F31" s="40" t="s">
+      <c r="F31" s="43" t="s">
         <v>36</v>
       </c>
       <c r="G31" s="26" t="s">
@@ -2641,56 +2659,56 @@
       <c r="H31" s="26" t="s">
         <v>38</v>
       </c>
-      <c r="I31" s="45" t="s">
+      <c r="I31" s="51" t="s">
         <v>39</v>
       </c>
       <c r="J31" s="26"/>
-      <c r="K31" s="47"/>
+      <c r="K31" s="53"/>
     </row>
     <row r="36" spans="1:1">
       <c r="A36" s="27" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="37" ht="17.25" spans="1:5">
+    <row r="37" spans="1:5">
       <c r="A37" s="28" t="s">
         <v>43</v>
       </c>
       <c r="B37" s="28"/>
       <c r="C37" s="28"/>
       <c r="D37" s="28"/>
-      <c r="E37" s="28"/>
+      <c r="E37" s="45"/>
     </row>
-    <row r="38" ht="17.25" spans="1:7">
+    <row r="38" ht="15.75" spans="1:7">
       <c r="A38" s="29" t="s">
         <v>44</v>
       </c>
       <c r="B38" s="29"/>
       <c r="C38" s="29"/>
       <c r="D38" s="29"/>
-      <c r="E38" s="29"/>
+      <c r="E38" s="46"/>
       <c r="F38" s="29"/>
       <c r="G38" s="29"/>
     </row>
-    <row r="39" ht="17.25" spans="1:7">
+    <row r="39" ht="15.75" spans="1:7">
       <c r="A39" s="29" t="s">
         <v>45</v>
       </c>
       <c r="B39" s="29"/>
       <c r="C39" s="29"/>
       <c r="D39" s="29"/>
-      <c r="E39" s="29"/>
+      <c r="E39" s="46"/>
       <c r="F39" s="29"/>
       <c r="G39" s="29"/>
     </row>
-    <row r="40" ht="16.5" spans="1:7">
+    <row r="40" spans="1:7">
       <c r="A40" s="30" t="s">
         <v>46</v>
       </c>
       <c r="B40" s="31"/>
       <c r="C40" s="31"/>
       <c r="D40" s="31"/>
-      <c r="E40" s="31"/>
+      <c r="E40" s="47"/>
       <c r="F40" s="31"/>
       <c r="G40" s="31"/>
     </row>
@@ -2737,7 +2755,7 @@
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
   <cols>
     <col min="16" max="17" width="13" customWidth="1"/>
-    <col min="18" max="19" width="13.5037037037037" customWidth="1"/>
+    <col min="18" max="19" width="13.5" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:19">

</xml_diff>